<commit_message>
Changes to Test data
</commit_message>
<xml_diff>
--- a/NewAccount/TestData/TestData.xlsx
+++ b/NewAccount/TestData/TestData.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diwakar.sharma.USCOFORGETECH\NewAccount\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diwakar.sharma.USCOFORGETECH\git\AccountCreation\NewAccount\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E80293F-9F6B-49EA-82DB-A5757886B7DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DADC8A-4709-482E-B334-A9C6D77C5B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateAccount" sheetId="3" r:id="rId1"/>
@@ -87,10 +87,10 @@
     <t>Mohan</t>
   </si>
   <si>
-    <t>test24@mail.com</t>
-  </si>
-  <si>
-    <t>test25@mail.com</t>
+    <t>test26@mail.com</t>
+  </si>
+  <si>
+    <t>test27@mail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Changes in Test data file
</commit_message>
<xml_diff>
--- a/NewAccount/TestData/TestData.xlsx
+++ b/NewAccount/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diwakar.sharma.USCOFORGETECH\git\AccountCreation\NewAccount\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3DADC8A-4709-482E-B334-A9C6D77C5B3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE56BB81-06A2-45D3-A6A0-92FABB7DAC84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -87,10 +87,10 @@
     <t>Mohan</t>
   </si>
   <si>
-    <t>test26@mail.com</t>
-  </si>
-  <si>
-    <t>test27@mail.com</t>
+    <t>test28@mail.com</t>
+  </si>
+  <si>
+    <t>test29@mail.com</t>
   </si>
 </sst>
 </file>
@@ -159,9 +159,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,34 +464,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -499,7 +499,7 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -520,10 +520,10 @@
       <c r="H2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -531,7 +531,7 @@
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -552,17 +552,17 @@
       <c r="H3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="J3" s="3" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{00BBB5C4-A323-4803-85C1-D7962C9CA8D8}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{EB0F08B8-3BC4-4FB9-8D3E-157B7EFFD22D}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{C8C7BD20-42EF-4189-B208-915FAA91B7B5}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{80CDE765-B4AA-425B-84B3-076C7B1A3F6E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>